<commit_message>
Regenerated the output folder based on the work completed in the master branch so far.
</commit_message>
<xml_diff>
--- a/output/flag-air-1.xlsx
+++ b/output/flag-air-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$42</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="284">
   <si>
     <t>Path</t>
   </si>
@@ -565,25 +565,73 @@
     <t>Flag.code</t>
   </si>
   <si>
+    <t>Coded or textual message to display to user</t>
+  </si>
+  <si>
+    <t>The coded value or textual component of the flag to display to the user.</t>
+  </si>
+  <si>
+    <t>If non coded, use CodeableConcept.text.  This element should always be included in the narrative.</t>
+  </si>
+  <si>
+    <t>Detail codes identifying specific flagged issues.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/flag-code</t>
+  </si>
+  <si>
+    <t>.value</t>
+  </si>
+  <si>
+    <t>what</t>
+  </si>
+  <si>
+    <t>Flag.code.id</t>
+  </si>
+  <si>
+    <t>Flag.code.extension</t>
+  </si>
+  <si>
+    <t>Flag.code.coding</t>
+  </si>
+  <si>
+    <t>Code defined by a terminology system</t>
+  </si>
+  <si>
+    <t>A reference to a code defined by a terminology system.</t>
+  </si>
+  <si>
+    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
+  </si>
+  <si>
+    <t>Allows for translations and alternate encodings within a code system.  Also supports communication of the same instance to systems requiring different encodings.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.coding</t>
+  </si>
+  <si>
+    <t>union(., ./translation)</t>
+  </si>
+  <si>
+    <t>Flag.code.text</t>
+  </si>
+  <si>
     <t>Notice text</t>
   </si>
   <si>
-    <t>The coded value or textual component of the flag to display to the user.</t>
-  </si>
-  <si>
-    <t>If non coded, use CodeableConcept.text.  This element should always be included in the narrative.</t>
-  </si>
-  <si>
-    <t>Detail codes identifying specific flagged issues.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/flag-code</t>
-  </si>
-  <si>
-    <t>.value</t>
-  </si>
-  <si>
-    <t>what</t>
+    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
+  </si>
+  <si>
+    <t>Very often the text is the same as a displayName of one of the codings.</t>
+  </si>
+  <si>
+    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
+  </si>
+  <si>
+    <t>CodeableConcept.text</t>
+  </si>
+  <si>
+    <t>./originalText[mediaType/code="text/plain"]/data</t>
   </si>
   <si>
     <t>Flag.subject</t>
@@ -1010,7 +1058,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK38"/>
+  <dimension ref="A1:AK42"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3261,7 +3309,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
         <v>181</v>
       </c>
@@ -3271,28 +3319,28 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>41</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>182</v>
+        <v>62</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>183</v>
+        <v>63</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>184</v>
+        <v>64</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3343,10 +3391,10 @@
         <v>41</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>181</v>
+        <v>65</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>48</v>
@@ -3358,26 +3406,26 @@
         <v>41</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>185</v>
+        <v>66</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>186</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>41</v>
@@ -3389,15 +3437,17 @@
         <v>41</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="M23" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>72</v>
+      </c>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>41</v>
@@ -3434,25 +3484,25 @@
         <v>41</v>
       </c>
       <c r="AA23" t="s" s="2">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="AC23" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD23" t="s" s="2">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>41</v>
@@ -3469,11 +3519,11 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -3489,21 +3539,23 @@
         <v>41</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>69</v>
+        <v>95</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>70</v>
+        <v>184</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>71</v>
+        <v>185</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="N24" s="2"/>
+        <v>186</v>
+      </c>
+      <c r="N24" t="s" s="2">
+        <v>187</v>
+      </c>
       <c r="O24" t="s" s="2">
         <v>41</v>
       </c>
@@ -3539,19 +3591,19 @@
         <v>41</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="AC24" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD24" t="s" s="2">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>76</v>
+        <v>188</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>39</v>
@@ -3566,7 +3618,7 @@
         <v>41</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>66</v>
+        <v>189</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>41</v>
@@ -3574,7 +3626,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3582,7 +3634,7 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F25" t="s" s="2">
         <v>48</v>
@@ -3600,15 +3652,17 @@
         <v>62</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="N25" s="2"/>
+        <v>193</v>
+      </c>
+      <c r="N25" t="s" s="2">
+        <v>194</v>
+      </c>
       <c r="O25" t="s" s="2">
         <v>41</v>
       </c>
@@ -3656,7 +3710,7 @@
         <v>41</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>39</v>
@@ -3665,21 +3719,21 @@
         <v>48</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>194</v>
+        <v>41</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>140</v>
+        <v>196</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="26" hidden="true">
+    <row r="26">
       <c r="A26" t="s" s="2">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3693,7 +3747,7 @@
         <v>48</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>41</v>
@@ -3702,17 +3756,15 @@
         <v>49</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>149</v>
+        <v>198</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>198</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>41</v>
@@ -3722,7 +3774,7 @@
         <v>41</v>
       </c>
       <c r="R26" t="s" s="2">
-        <v>199</v>
+        <v>41</v>
       </c>
       <c r="S26" t="s" s="2">
         <v>41</v>
@@ -3761,10 +3813,10 @@
         <v>41</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>48</v>
@@ -3779,12 +3831,12 @@
         <v>201</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>41</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3887,7 +3939,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -3992,7 +4044,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4009,26 +4061,24 @@
         <v>41</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I29" t="s" s="2">
         <v>49</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>117</v>
+        <v>62</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="N29" t="s" s="2">
         <v>208</v>
       </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>41</v>
       </c>
@@ -4052,46 +4102,46 @@
         <v>41</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>159</v>
+        <v>41</v>
       </c>
       <c r="X29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE29" t="s" s="2">
         <v>209</v>
       </c>
-      <c r="Y29" t="s" s="2">
+      <c r="AF29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH29" t="s" s="2">
         <v>210</v>
       </c>
-      <c r="Z29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE29" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="AF29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="AI29" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>212</v>
+        <v>140</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>41</v>
@@ -4099,7 +4149,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4107,7 +4157,7 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>48</v>
@@ -4122,20 +4172,18 @@
         <v>49</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="K30" t="s" s="2">
+        <v>212</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="M30" t="s" s="2">
         <v>214</v>
       </c>
-      <c r="L30" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>217</v>
-      </c>
+      <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
         <v>41</v>
       </c>
@@ -4144,7 +4192,7 @@
         <v>41</v>
       </c>
       <c r="R30" t="s" s="2">
-        <v>41</v>
+        <v>215</v>
       </c>
       <c r="S30" t="s" s="2">
         <v>41</v>
@@ -4159,13 +4207,13 @@
         <v>41</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>218</v>
+        <v>41</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>219</v>
+        <v>41</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>41</v>
@@ -4183,7 +4231,7 @@
         <v>41</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>39</v>
@@ -4198,7 +4246,7 @@
         <v>41</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>212</v>
+        <v>217</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>41</v>
@@ -4206,7 +4254,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4226,21 +4274,19 @@
         <v>41</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>222</v>
+        <v>63</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>223</v>
+        <v>64</v>
       </c>
       <c r="M31" s="2"/>
-      <c r="N31" t="s" s="2">
-        <v>224</v>
-      </c>
+      <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>41</v>
       </c>
@@ -4252,7 +4298,7 @@
         <v>41</v>
       </c>
       <c r="S31" t="s" s="2">
-        <v>225</v>
+        <v>41</v>
       </c>
       <c r="T31" t="s" s="2">
         <v>41</v>
@@ -4288,7 +4334,7 @@
         <v>41</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>226</v>
+        <v>65</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>39</v>
@@ -4303,7 +4349,7 @@
         <v>41</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>227</v>
+        <v>66</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>41</v>
@@ -4311,18 +4357,18 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>41</v>
@@ -4331,19 +4377,19 @@
         <v>41</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>229</v>
+        <v>70</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>230</v>
+        <v>71</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>231</v>
+        <v>72</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -4357,7 +4403,7 @@
         <v>41</v>
       </c>
       <c r="S32" t="s" s="2">
-        <v>232</v>
+        <v>41</v>
       </c>
       <c r="T32" t="s" s="2">
         <v>41</v>
@@ -4381,25 +4427,25 @@
         <v>41</v>
       </c>
       <c r="AA32" t="s" s="2">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="AB32" t="s" s="2">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="AC32" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD32" t="s" s="2">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>233</v>
+        <v>76</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>41</v>
@@ -4408,7 +4454,7 @@
         <v>41</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>234</v>
+        <v>66</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>41</v>
@@ -4416,7 +4462,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4433,22 +4479,26 @@
         <v>41</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I33" t="s" s="2">
         <v>49</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>236</v>
+        <v>117</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+        <v>222</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="N33" t="s" s="2">
+        <v>224</v>
+      </c>
       <c r="O33" t="s" s="2">
         <v>41</v>
       </c>
@@ -4472,13 +4522,13 @@
         <v>41</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>41</v>
+        <v>159</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>41</v>
+        <v>225</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>41</v>
+        <v>226</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>41</v>
@@ -4496,7 +4546,7 @@
         <v>41</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>39</v>
@@ -4511,7 +4561,7 @@
         <v>41</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>41</v>
@@ -4519,7 +4569,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4542,18 +4592,20 @@
         <v>49</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>242</v>
+        <v>165</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="N34" s="2"/>
+        <v>232</v>
+      </c>
+      <c r="N34" t="s" s="2">
+        <v>233</v>
+      </c>
       <c r="O34" t="s" s="2">
         <v>41</v>
       </c>
@@ -4577,13 +4629,13 @@
         <v>41</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>41</v>
+        <v>234</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>41</v>
+        <v>235</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>41</v>
@@ -4601,7 +4653,7 @@
         <v>41</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>39</v>
@@ -4616,7 +4668,7 @@
         <v>41</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>247</v>
+        <v>228</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>41</v>
@@ -4624,7 +4676,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4647,18 +4699,18 @@
         <v>49</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="N35" s="2"/>
+        <v>239</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" t="s" s="2">
+        <v>240</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>41</v>
       </c>
@@ -4670,7 +4722,7 @@
         <v>41</v>
       </c>
       <c r="S35" t="s" s="2">
-        <v>41</v>
+        <v>241</v>
       </c>
       <c r="T35" t="s" s="2">
         <v>41</v>
@@ -4706,7 +4758,7 @@
         <v>41</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>39</v>
@@ -4721,7 +4773,7 @@
         <v>41</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>140</v>
+        <v>243</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>41</v>
@@ -4729,7 +4781,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4737,7 +4789,7 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F36" t="s" s="2">
         <v>48</v>
@@ -4752,15 +4804,17 @@
         <v>49</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>236</v>
+        <v>62</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="M36" s="2"/>
+        <v>246</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>247</v>
+      </c>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>41</v>
@@ -4773,7 +4827,7 @@
         <v>41</v>
       </c>
       <c r="S36" t="s" s="2">
-        <v>41</v>
+        <v>248</v>
       </c>
       <c r="T36" t="s" s="2">
         <v>41</v>
@@ -4809,7 +4863,7 @@
         <v>41</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>39</v>
@@ -4824,15 +4878,15 @@
         <v>41</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>41</v>
+        <v>250</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>256</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -4855,17 +4909,15 @@
         <v>49</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>261</v>
-      </c>
+        <v>254</v>
+      </c>
+      <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>41</v>
@@ -4914,7 +4966,7 @@
         <v>41</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>39</v>
@@ -4929,15 +4981,15 @@
         <v>41</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>41</v>
+        <v>256</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>256</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -4960,15 +5012,17 @@
         <v>49</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="M38" s="2"/>
+        <v>260</v>
+      </c>
+      <c r="M38" t="s" s="2">
+        <v>261</v>
+      </c>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>41</v>
@@ -5032,14 +5086,430 @@
         <v>41</v>
       </c>
       <c r="AJ38" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="AK38" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" hidden="true">
+      <c r="A39" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F39" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I39" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J39" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="K39" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="L39" t="s" s="2">
         <v>266</v>
       </c>
-      <c r="AK38" t="s" s="2">
+      <c r="M39" t="s" s="2">
         <v>267</v>
+      </c>
+      <c r="N39" s="2"/>
+      <c r="O39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P39" s="2"/>
+      <c r="Q39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE39" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="AF39" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG39" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ39" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="AK39" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" hidden="true">
+      <c r="A40" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F40" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I40" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J40" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P40" s="2"/>
+      <c r="Q40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE40" t="s" s="2">
+        <v>269</v>
+      </c>
+      <c r="AF40" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG40" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="41" hidden="true">
+      <c r="A41" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F41" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I41" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J41" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="K41" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="L41" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="N41" s="2"/>
+      <c r="O41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P41" s="2"/>
+      <c r="Q41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE41" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="AF41" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG41" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="42" hidden="true">
+      <c r="A42" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="B42" s="2"/>
+      <c r="C42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D42" s="2"/>
+      <c r="E42" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F42" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="G42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I42" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="J42" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="K42" t="s" s="2">
+        <v>280</v>
+      </c>
+      <c r="L42" t="s" s="2">
+        <v>281</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P42" s="2"/>
+      <c r="Q42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE42" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="AF42" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG42" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI42" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ42" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="AK42" t="s" s="2">
+        <v>283</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK38">
+  <autoFilter ref="A1:AK42">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5049,7 +5519,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI37">
+  <conditionalFormatting sqref="A2:AI41">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
FHIR IG with updated profile status and improved profile intro content
</commit_message>
<xml_diff>
--- a/output/flag-air-1.xlsx
+++ b/output/flag-air-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$38</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="268">
   <si>
     <t>Path</t>
   </si>
@@ -584,54 +584,6 @@
   </si>
   <si>
     <t>what</t>
-  </si>
-  <si>
-    <t>Flag.code.id</t>
-  </si>
-  <si>
-    <t>Flag.code.extension</t>
-  </si>
-  <si>
-    <t>Flag.code.coding</t>
-  </si>
-  <si>
-    <t>Code defined by a terminology system</t>
-  </si>
-  <si>
-    <t>A reference to a code defined by a terminology system.</t>
-  </si>
-  <si>
-    <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
-  </si>
-  <si>
-    <t>Allows for translations and alternate encodings within a code system.  Also supports communication of the same instance to systems requiring different encodings.</t>
-  </si>
-  <si>
-    <t>CodeableConcept.coding</t>
-  </si>
-  <si>
-    <t>union(., ./translation)</t>
-  </si>
-  <si>
-    <t>Flag.code.text</t>
-  </si>
-  <si>
-    <t>Notice text</t>
-  </si>
-  <si>
-    <t>A human language representation of the concept as seen/selected/uttered by the user who entered the data and/or which represents the intended meaning of the user.</t>
-  </si>
-  <si>
-    <t>Very often the text is the same as a displayName of one of the codings.</t>
-  </si>
-  <si>
-    <t>The codes from the terminologies do not always capture the correct meaning with all the nuances of the human using them, or sometimes there is no appropriate code at all. In these cases, the text is used to capture the full meaning of the source.</t>
-  </si>
-  <si>
-    <t>CodeableConcept.text</t>
-  </si>
-  <si>
-    <t>./originalText[mediaType/code="text/plain"]/data</t>
   </si>
   <si>
     <t>Flag.subject</t>
@@ -1058,7 +1010,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK42"/>
+  <dimension ref="A1:AK38"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -3309,7 +3261,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
         <v>181</v>
       </c>
@@ -3319,28 +3271,28 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F22" t="s" s="2">
         <v>48</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>41</v>
       </c>
       <c r="I22" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>62</v>
+        <v>182</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>63</v>
+        <v>183</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>64</v>
+        <v>184</v>
       </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -3391,10 +3343,10 @@
         <v>41</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>65</v>
+        <v>181</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>48</v>
@@ -3406,26 +3358,26 @@
         <v>41</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>66</v>
+        <v>185</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>41</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>41</v>
@@ -3437,17 +3389,15 @@
         <v>41</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>72</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>41</v>
@@ -3484,25 +3434,25 @@
         <v>41</v>
       </c>
       <c r="AA23" t="s" s="2">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="AB23" t="s" s="2">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="AC23" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD23" t="s" s="2">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>41</v>
@@ -3519,11 +3469,11 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -3539,23 +3489,21 @@
         <v>41</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>184</v>
+        <v>70</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>185</v>
+        <v>71</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>187</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
         <v>41</v>
       </c>
@@ -3591,19 +3539,19 @@
         <v>41</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="AC24" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD24" t="s" s="2">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>188</v>
+        <v>76</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>39</v>
@@ -3618,7 +3566,7 @@
         <v>41</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>189</v>
+        <v>66</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>41</v>
@@ -3626,7 +3574,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3634,7 +3582,7 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F25" t="s" s="2">
         <v>48</v>
@@ -3652,17 +3600,15 @@
         <v>62</v>
       </c>
       <c r="K25" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="L25" t="s" s="2">
         <v>191</v>
       </c>
-      <c r="L25" t="s" s="2">
+      <c r="M25" t="s" s="2">
         <v>192</v>
       </c>
-      <c r="M25" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>194</v>
-      </c>
+      <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>41</v>
       </c>
@@ -3710,30 +3656,30 @@
         <v>41</v>
       </c>
       <c r="AE25" t="s" s="2">
+        <v>193</v>
+      </c>
+      <c r="AF25" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG25" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="AH25" t="s" s="2">
+        <v>194</v>
+      </c>
+      <c r="AI25" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ25" t="s" s="2">
+        <v>140</v>
+      </c>
+      <c r="AK25" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" hidden="true">
+      <c r="A26" t="s" s="2">
         <v>195</v>
-      </c>
-      <c r="AF25" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG25" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH25" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI25" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ25" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="AK25" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s" s="2">
-        <v>197</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3747,7 +3693,7 @@
         <v>48</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>41</v>
@@ -3756,15 +3702,17 @@
         <v>49</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>149</v>
+      </c>
+      <c r="K26" t="s" s="2">
+        <v>196</v>
+      </c>
+      <c r="L26" t="s" s="2">
+        <v>197</v>
+      </c>
+      <c r="M26" t="s" s="2">
         <v>198</v>
       </c>
-      <c r="K26" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="M26" s="2"/>
       <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>41</v>
@@ -3774,7 +3722,7 @@
         <v>41</v>
       </c>
       <c r="R26" t="s" s="2">
-        <v>41</v>
+        <v>199</v>
       </c>
       <c r="S26" t="s" s="2">
         <v>41</v>
@@ -3813,10 +3761,10 @@
         <v>41</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>48</v>
@@ -3831,12 +3779,12 @@
         <v>201</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>202</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3939,7 +3887,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4044,7 +3992,7 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4061,24 +4009,26 @@
         <v>41</v>
       </c>
       <c r="H29" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="I29" t="s" s="2">
         <v>49</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="K29" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="L29" t="s" s="2">
         <v>206</v>
       </c>
-      <c r="L29" t="s" s="2">
+      <c r="M29" t="s" s="2">
         <v>207</v>
       </c>
-      <c r="M29" t="s" s="2">
+      <c r="N29" t="s" s="2">
         <v>208</v>
       </c>
-      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>41</v>
       </c>
@@ -4102,13 +4052,13 @@
         <v>41</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>41</v>
+        <v>159</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>41</v>
+        <v>209</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>41</v>
+        <v>210</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>41</v>
@@ -4126,7 +4076,7 @@
         <v>41</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>39</v>
@@ -4135,13 +4085,13 @@
         <v>48</v>
       </c>
       <c r="AH29" t="s" s="2">
-        <v>210</v>
+        <v>41</v>
       </c>
       <c r="AI29" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ29" t="s" s="2">
-        <v>140</v>
+        <v>212</v>
       </c>
       <c r="AK29" t="s" s="2">
         <v>41</v>
@@ -4149,7 +4099,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4157,7 +4107,7 @@
       </c>
       <c r="D30" s="2"/>
       <c r="E30" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F30" t="s" s="2">
         <v>48</v>
@@ -4172,18 +4122,20 @@
         <v>49</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>149</v>
+        <v>165</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="N30" s="2"/>
+        <v>216</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>217</v>
+      </c>
       <c r="O30" t="s" s="2">
         <v>41</v>
       </c>
@@ -4192,7 +4144,7 @@
         <v>41</v>
       </c>
       <c r="R30" t="s" s="2">
-        <v>215</v>
+        <v>41</v>
       </c>
       <c r="S30" t="s" s="2">
         <v>41</v>
@@ -4207,13 +4159,13 @@
         <v>41</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>41</v>
+        <v>218</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>41</v>
+        <v>219</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>41</v>
@@ -4231,7 +4183,7 @@
         <v>41</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>39</v>
@@ -4246,7 +4198,7 @@
         <v>41</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="AK30" t="s" s="2">
         <v>41</v>
@@ -4254,7 +4206,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -4274,19 +4226,21 @@
         <v>41</v>
       </c>
       <c r="I31" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>63</v>
+        <v>222</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>64</v>
+        <v>223</v>
       </c>
       <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+      <c r="N31" t="s" s="2">
+        <v>224</v>
+      </c>
       <c r="O31" t="s" s="2">
         <v>41</v>
       </c>
@@ -4298,7 +4252,7 @@
         <v>41</v>
       </c>
       <c r="S31" t="s" s="2">
-        <v>41</v>
+        <v>225</v>
       </c>
       <c r="T31" t="s" s="2">
         <v>41</v>
@@ -4334,7 +4288,7 @@
         <v>41</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>65</v>
+        <v>226</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>39</v>
@@ -4349,7 +4303,7 @@
         <v>41</v>
       </c>
       <c r="AJ31" t="s" s="2">
-        <v>66</v>
+        <v>227</v>
       </c>
       <c r="AK31" t="s" s="2">
         <v>41</v>
@@ -4357,18 +4311,18 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D32" s="2"/>
       <c r="E32" t="s" s="2">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>41</v>
@@ -4377,19 +4331,19 @@
         <v>41</v>
       </c>
       <c r="I32" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>70</v>
+        <v>229</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>71</v>
+        <v>230</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>72</v>
+        <v>231</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
@@ -4403,7 +4357,7 @@
         <v>41</v>
       </c>
       <c r="S32" t="s" s="2">
-        <v>41</v>
+        <v>232</v>
       </c>
       <c r="T32" t="s" s="2">
         <v>41</v>
@@ -4427,25 +4381,25 @@
         <v>41</v>
       </c>
       <c r="AA32" t="s" s="2">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="AB32" t="s" s="2">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="AC32" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD32" t="s" s="2">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>76</v>
+        <v>233</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>41</v>
@@ -4454,7 +4408,7 @@
         <v>41</v>
       </c>
       <c r="AJ32" t="s" s="2">
-        <v>66</v>
+        <v>234</v>
       </c>
       <c r="AK32" t="s" s="2">
         <v>41</v>
@@ -4462,7 +4416,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -4479,26 +4433,22 @@
         <v>41</v>
       </c>
       <c r="H33" t="s" s="2">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="I33" t="s" s="2">
         <v>49</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>117</v>
+        <v>236</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="N33" t="s" s="2">
-        <v>224</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>41</v>
       </c>
@@ -4522,13 +4472,13 @@
         <v>41</v>
       </c>
       <c r="W33" t="s" s="2">
-        <v>159</v>
+        <v>41</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>225</v>
+        <v>41</v>
       </c>
       <c r="Y33" t="s" s="2">
-        <v>226</v>
+        <v>41</v>
       </c>
       <c r="Z33" t="s" s="2">
         <v>41</v>
@@ -4546,7 +4496,7 @@
         <v>41</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>39</v>
@@ -4561,7 +4511,7 @@
         <v>41</v>
       </c>
       <c r="AJ33" t="s" s="2">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="AK33" t="s" s="2">
         <v>41</v>
@@ -4569,7 +4519,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -4592,20 +4542,18 @@
         <v>49</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>165</v>
+        <v>242</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>233</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>41</v>
       </c>
@@ -4629,13 +4577,13 @@
         <v>41</v>
       </c>
       <c r="W34" t="s" s="2">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="X34" t="s" s="2">
-        <v>234</v>
+        <v>41</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>235</v>
+        <v>41</v>
       </c>
       <c r="Z34" t="s" s="2">
         <v>41</v>
@@ -4653,7 +4601,7 @@
         <v>41</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>39</v>
@@ -4668,7 +4616,7 @@
         <v>41</v>
       </c>
       <c r="AJ34" t="s" s="2">
-        <v>228</v>
+        <v>247</v>
       </c>
       <c r="AK34" t="s" s="2">
         <v>41</v>
@@ -4676,7 +4624,7 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>237</v>
+        <v>248</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
@@ -4699,18 +4647,18 @@
         <v>49</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" t="s" s="2">
-        <v>240</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>41</v>
       </c>
@@ -4722,7 +4670,7 @@
         <v>41</v>
       </c>
       <c r="S35" t="s" s="2">
-        <v>241</v>
+        <v>41</v>
       </c>
       <c r="T35" t="s" s="2">
         <v>41</v>
@@ -4758,7 +4706,7 @@
         <v>41</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>242</v>
+        <v>252</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>39</v>
@@ -4773,7 +4721,7 @@
         <v>41</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>243</v>
+        <v>140</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>41</v>
@@ -4781,7 +4729,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -4789,7 +4737,7 @@
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F36" t="s" s="2">
         <v>48</v>
@@ -4804,17 +4752,15 @@
         <v>49</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>62</v>
+        <v>236</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>247</v>
-      </c>
+        <v>255</v>
+      </c>
+      <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" t="s" s="2">
         <v>41</v>
@@ -4827,7 +4773,7 @@
         <v>41</v>
       </c>
       <c r="S36" t="s" s="2">
-        <v>248</v>
+        <v>41</v>
       </c>
       <c r="T36" t="s" s="2">
         <v>41</v>
@@ -4863,7 +4809,7 @@
         <v>41</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>39</v>
@@ -4878,15 +4824,15 @@
         <v>41</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>250</v>
+        <v>41</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>41</v>
+        <v>256</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -4909,15 +4855,17 @@
         <v>49</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="M37" s="2"/>
+        <v>260</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>261</v>
+      </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>41</v>
@@ -4966,7 +4914,7 @@
         <v>41</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>39</v>
@@ -4981,15 +4929,15 @@
         <v>41</v>
       </c>
       <c r="AJ37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AK37" t="s" s="2">
         <v>256</v>
-      </c>
-      <c r="AK37" t="s" s="2">
-        <v>41</v>
       </c>
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5012,17 +4960,15 @@
         <v>49</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>261</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>41</v>
@@ -5086,430 +5032,14 @@
         <v>41</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39" hidden="true">
-      <c r="A39" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F39" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I39" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J39" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="K39" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="M39" t="s" s="2">
         <v>267</v>
-      </c>
-      <c r="N39" s="2"/>
-      <c r="O39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P39" s="2"/>
-      <c r="Q39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE39" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="AF39" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG39" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ39" t="s" s="2">
-        <v>140</v>
-      </c>
-      <c r="AK39" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="40" hidden="true">
-      <c r="A40" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F40" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I40" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J40" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="K40" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P40" s="2"/>
-      <c r="Q40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="AF40" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG40" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="41" hidden="true">
-      <c r="A41" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F41" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I41" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J41" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="K41" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="N41" s="2"/>
-      <c r="O41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P41" s="2"/>
-      <c r="Q41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE41" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="AF41" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG41" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK41" t="s" s="2">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="42" hidden="true">
-      <c r="A42" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D42" s="2"/>
-      <c r="E42" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F42" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I42" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J42" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="K42" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="L42" t="s" s="2">
-        <v>281</v>
-      </c>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P42" s="2"/>
-      <c r="Q42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE42" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="AF42" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG42" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI42" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ42" t="s" s="2">
-        <v>282</v>
-      </c>
-      <c r="AK42" t="s" s="2">
-        <v>283</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK42">
+  <autoFilter ref="A1:AK38">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5519,7 +5049,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI41">
+  <conditionalFormatting sqref="A2:AI37">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated commented out content from AIR Immunisation & AIR Notice StructureDefinition files
</commit_message>
<xml_diff>
--- a/output/flag-air-1.xlsx
+++ b/output/flag-air-1.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$25</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="203">
   <si>
     <t>Path</t>
   </si>
@@ -605,219 +605,11 @@
     <t>who.focus</t>
   </si>
   <si>
-    <t>Flag.subject.id</t>
-  </si>
-  <si>
-    <t>Flag.subject.extension</t>
-  </si>
-  <si>
-    <t>Flag.subject.reference</t>
-  </si>
-  <si>
-    <t>Literal reference, Relative, internal or absolute URL</t>
-  </si>
-  <si>
-    <t>A reference to a location at which the other resource is found. The reference may be a relative reference, in which case it is relative to the service base URL, or an absolute URL that resolves to the location where the resource is found. The reference may be version specific or not. If the reference is not to a FHIR RESTful server, then it should be assumed to be version specific. Internal fragment references (start with '#') refer to contained resources.</t>
-  </si>
-  <si>
-    <t>Using absolute URLs provides a stable scalable approach suitable for a cloud/web context, while using relative/logical references provides a flexible approach suitable for use when trading across closed eco-system boundaries.   Absolute URLs do not need to point to a FHIR RESTful server, though this is the preferred approach. If the URL conforms to the structure "/[type]/[id]" then it should be assumed that the reference is to a FHIR RESTful server.</t>
-  </si>
-  <si>
-    <t>Reference.reference</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ref-1
-</t>
-  </si>
-  <si>
-    <t>Flag.subject.identifier</t>
-  </si>
-  <si>
-    <t>Individual Healthcare Identifier (IHI)</t>
-  </si>
-  <si>
-    <t>An identifier for the other resource. This is used when there is no way to reference the other resource directly, either because the entity is not available through a FHIR server, or because there is no way for the author of the resource to convert a known identifier to an actual location. There is no requirement that a Reference.identifier point to something that is actually exposed as a FHIR instance, but it SHALL point to a business concept that would be expected to be exposed as a FHIR instance, and that instance would need to be of a FHIR resource type allowed by the reference.</t>
-  </si>
-  <si>
-    <t>When an identifier is provided in place of a reference, any system processing the reference will only be able to resolve the identifier to a reference if it understands the business context in which the identifier is used. Sometimes this is global (e.g. a national identifier) but often it is not. For this reason, none of the useful mechanisms described for working with references (e.g. chaining, includes) are possible, nor should servers be expected to be able resolve the reference. Servers may accept an identifier based reference untouched, resolve it, and/or reject it - see CapabilityStatement.rest.resource.referencePolicy. 
-When both an identifier and a literal reference are provided, the literal reference is preferred. Applications processing the resource are allowed - but not required - to check that the identifier matches the literal reference
-Applications converting a logical reference to a literal reference may choose to leave the logical reference present, or remove it.</t>
-  </si>
-  <si>
-    <t>&lt;valueIdentifier xmlns="http://hl7.org/fhir"&gt;
-  &lt;type&gt;
-    &lt;coding&gt;
-      &lt;system value="http://hl7.org/fhir/v2/0203"/&gt;
-      &lt;code value="NI"/&gt;
-    &lt;/coding&gt;
-  &lt;/type&gt;
-  &lt;system value="http://ns.electronichealth.net.au/id/hi/ihi/1.0"/&gt;
-&lt;/valueIdentifier&gt;</t>
-  </si>
-  <si>
-    <t>Reference.identifier</t>
-  </si>
-  <si>
-    <t>.identifier</t>
-  </si>
-  <si>
-    <t>Flag.subject.identifier.id</t>
-  </si>
-  <si>
-    <t>Flag.subject.identifier.extension</t>
-  </si>
-  <si>
-    <t>Flag.subject.identifier.use</t>
-  </si>
-  <si>
-    <t>usual | official | temp | secondary (If known)</t>
-  </si>
-  <si>
-    <t>The purpose of this identifier.</t>
-  </si>
-  <si>
-    <t>This is labeled as "Is Modifier" because applications should not mistake a temporary id for a permanent one. Applications can assume that an identifier is permanent unless it explicitly says that it is temporary.</t>
-  </si>
-  <si>
-    <t>Allows the appropriate identifier for a particular context of use to be selected from among a set of identifiers.</t>
-  </si>
-  <si>
-    <t>Identifies the purpose for this identifier, if known .</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/identifier-use</t>
-  </si>
-  <si>
-    <t>Identifier.use</t>
-  </si>
-  <si>
-    <t>Role.code or implied by context</t>
-  </si>
-  <si>
-    <t>Flag.subject.identifier.type</t>
-  </si>
-  <si>
-    <t>Description of identifier</t>
-  </si>
-  <si>
-    <t>A coded type for the identifier that can be used to determine which identifier to use for a specific purpose.</t>
-  </si>
-  <si>
-    <t>This element deals only with general categories of identifiers.  It SHOULD not be used for codes that correspond 1..1 with the Identifier.system. Some identifiers may fall into multiple categories due to common usage. 
-Where the system is known, a type is unnecessary because the type is always part of the system definition. However systems often need to handle identifiers where the system is not known. There is not a 1:1 relationship between type and system, since many different systems have the same type.</t>
-  </si>
-  <si>
-    <t>Allows users to make use of identifiers when the identifier system is not known.</t>
-  </si>
-  <si>
-    <t>A coded type for an identifier that can be used to determine which identifier to use for a specific purpose.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/identifier-type</t>
-  </si>
-  <si>
-    <t>Identifier.type</t>
-  </si>
-  <si>
-    <t>Flag.subject.identifier.system</t>
-  </si>
-  <si>
-    <t>The namespace for the identifier value</t>
-  </si>
-  <si>
-    <t>Establishes the namespace for the value - that is, a URL that describes a set values that are unique.</t>
-  </si>
-  <si>
-    <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
-  </si>
-  <si>
-    <t>http://www.acme.com/identifiers/patient</t>
-  </si>
-  <si>
-    <t>Identifier.system</t>
-  </si>
-  <si>
-    <t>II.root or Role.id.root</t>
-  </si>
-  <si>
-    <t>Flag.subject.identifier.value</t>
-  </si>
-  <si>
-    <t>IHI</t>
-  </si>
-  <si>
-    <t>The portion of the identifier typically relevant to the user and which is unique within the context of the system.</t>
-  </si>
-  <si>
-    <t>If the value is a full URI, then the system SHALL be urn:ietf:rfc:3986.  The value's primary purpose is computational mapping.  As a result, it may be normalized for comparison purposes (e.g. removing non-significant whitespace, dashes, etc.)  A value formatted for human display can be conveyed using the [Rendered Value extension](http://hl7.org/fhir/STU3/extension-rendered-value.html).</t>
-  </si>
-  <si>
-    <t>123456</t>
-  </si>
-  <si>
-    <t>Identifier.value</t>
-  </si>
-  <si>
-    <t>II.extension or II.root if system indicates OID or GUID (Or Role.id.extension or root)</t>
-  </si>
-  <si>
-    <t>Flag.subject.identifier.period</t>
+    <t>Flag.period</t>
   </si>
   <si>
     <t xml:space="preserve">Period
 </t>
-  </si>
-  <si>
-    <t>Time period when id is/was valid for use</t>
-  </si>
-  <si>
-    <t>Time period during which identifier is/was valid for use.</t>
-  </si>
-  <si>
-    <t>Identifier.period</t>
-  </si>
-  <si>
-    <t>Role.effectiveTime or implied by context</t>
-  </si>
-  <si>
-    <t>Flag.subject.identifier.assigner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference(Organization)
-</t>
-  </si>
-  <si>
-    <t>Organization that issued id (may be just text)</t>
-  </si>
-  <si>
-    <t>Organization that issued/manages the identifier.</t>
-  </si>
-  <si>
-    <t>The Identifier.assigner may omit the .reference element and only contain a .display element reflecting the name or other textual information about the assigning organization.</t>
-  </si>
-  <si>
-    <t>Identifier.assigner</t>
-  </si>
-  <si>
-    <t>II.assigningAuthorityName but note that this is an improper use by the definition of the field.  Also Role.scoper</t>
-  </si>
-  <si>
-    <t>Flag.subject.display</t>
-  </si>
-  <si>
-    <t>Text alternative for the resource</t>
-  </si>
-  <si>
-    <t>Plain text narrative that identifies the resource in addition to the resource reference.</t>
-  </si>
-  <si>
-    <t>This is generally not the same as the Resource.text of the referenced resource.  The purpose is to identify what's being referenced, not to fully describe it.</t>
-  </si>
-  <si>
-    <t>Reference.display</t>
-  </si>
-  <si>
-    <t>Flag.period</t>
   </si>
   <si>
     <t>Time period when flag is active</t>
@@ -1010,7 +802,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK38"/>
+  <dimension ref="A1:AK25"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1019,7 +811,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="29.67578125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="21.5078125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
@@ -1054,7 +846,7 @@
     <col min="33" max="33" width="9.875" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.21875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="99.6875" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="63.46484375" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="22.03125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -3386,16 +3178,16 @@
         <v>41</v>
       </c>
       <c r="I23" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>62</v>
+        <v>188</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>63</v>
+        <v>189</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>64</v>
+        <v>190</v>
       </c>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -3446,7 +3238,7 @@
         <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>65</v>
+        <v>187</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>39</v>
@@ -3461,26 +3253,26 @@
         <v>41</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>41</v>
+        <v>191</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>68</v>
+        <v>41</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>41</v>
@@ -3489,19 +3281,19 @@
         <v>41</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>69</v>
+        <v>193</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>70</v>
+        <v>194</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>71</v>
+        <v>195</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>72</v>
+        <v>196</v>
       </c>
       <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
@@ -3539,25 +3331,25 @@
         <v>41</v>
       </c>
       <c r="AA24" t="s" s="2">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="AC24" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD24" t="s" s="2">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>76</v>
+        <v>192</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH24" t="s" s="2">
         <v>41</v>
@@ -3566,15 +3358,15 @@
         <v>41</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>41</v>
+        <v>191</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3597,17 +3389,15 @@
         <v>49</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>62</v>
+        <v>198</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>192</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="M25" s="2"/>
       <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>41</v>
@@ -3656,7 +3446,7 @@
         <v>41</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>39</v>
@@ -3665,1381 +3455,20 @@
         <v>48</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>194</v>
+        <v>41</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>140</v>
+        <v>201</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="26" hidden="true">
-      <c r="A26" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D26" s="2"/>
-      <c r="E26" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="F26" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I26" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J26" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="K26" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="L26" t="s" s="2">
-        <v>197</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>198</v>
-      </c>
-      <c r="N26" s="2"/>
-      <c r="O26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P26" s="2"/>
-      <c r="Q26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R26" t="s" s="2">
-        <v>199</v>
-      </c>
-      <c r="S26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE26" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="AF26" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG26" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI26" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ26" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="AK26" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" hidden="true">
-      <c r="A27" t="s" s="2">
         <v>202</v>
-      </c>
-      <c r="B27" s="2"/>
-      <c r="C27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F27" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J27" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="K27" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="L27" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P27" s="2"/>
-      <c r="Q27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE27" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="AF27" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG27" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ27" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="AK27" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" hidden="true">
-      <c r="A28" t="s" s="2">
-        <v>203</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F28" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="G28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J28" t="s" s="2">
-        <v>69</v>
-      </c>
-      <c r="K28" t="s" s="2">
-        <v>70</v>
-      </c>
-      <c r="L28" t="s" s="2">
-        <v>71</v>
-      </c>
-      <c r="M28" t="s" s="2">
-        <v>72</v>
-      </c>
-      <c r="N28" s="2"/>
-      <c r="O28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P28" s="2"/>
-      <c r="Q28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA28" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="AB28" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="AC28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD28" t="s" s="2">
-        <v>75</v>
-      </c>
-      <c r="AE28" t="s" s="2">
-        <v>76</v>
-      </c>
-      <c r="AF28" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG28" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ28" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="AK28" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" hidden="true">
-      <c r="A29" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F29" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H29" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="I29" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J29" t="s" s="2">
-        <v>117</v>
-      </c>
-      <c r="K29" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="O29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P29" s="2"/>
-      <c r="Q29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W29" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="X29" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="Y29" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="Z29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE29" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="AF29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="AK29" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" hidden="true">
-      <c r="A30" t="s" s="2">
-        <v>213</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F30" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I30" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J30" t="s" s="2">
-        <v>165</v>
-      </c>
-      <c r="K30" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="O30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P30" s="2"/>
-      <c r="Q30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W30" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="X30" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="Y30" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="Z30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE30" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="AF30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG30" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ30" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="AK30" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" hidden="true">
-      <c r="A31" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F31" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I31" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J31" t="s" s="2">
-        <v>89</v>
-      </c>
-      <c r="K31" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="M31" s="2"/>
-      <c r="N31" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="O31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P31" s="2"/>
-      <c r="Q31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S31" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="T31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE31" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="AF31" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG31" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ31" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" hidden="true">
-      <c r="A32" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="F32" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I32" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J32" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="K32" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="N32" s="2"/>
-      <c r="O32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P32" s="2"/>
-      <c r="Q32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S32" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="T32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE32" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="AF32" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG32" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ32" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="AK32" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" hidden="true">
-      <c r="A33" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F33" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I33" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J33" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="K33" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P33" s="2"/>
-      <c r="Q33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE33" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="AF33" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG33" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ33" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="AK33" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" hidden="true">
-      <c r="A34" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F34" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I34" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J34" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="K34" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="N34" s="2"/>
-      <c r="O34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P34" s="2"/>
-      <c r="Q34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE34" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="AF34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG34" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="AK34" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35" hidden="true">
-      <c r="A35" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F35" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I35" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J35" t="s" s="2">
-        <v>62</v>
-      </c>
-      <c r="K35" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="M35" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="N35" s="2"/>
-      <c r="O35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P35" s="2"/>
-      <c r="Q35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE35" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="AF35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG35" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ35" t="s" s="2">
-        <v>140</v>
-      </c>
-      <c r="AK35" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" hidden="true">
-      <c r="A36" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F36" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I36" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J36" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="K36" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P36" s="2"/>
-      <c r="Q36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE36" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="AF36" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG36" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK36" t="s" s="2">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="37" hidden="true">
-      <c r="A37" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F37" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I37" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J37" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="K37" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="N37" s="2"/>
-      <c r="O37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P37" s="2"/>
-      <c r="Q37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE37" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="AF37" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG37" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AK37" t="s" s="2">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="38" hidden="true">
-      <c r="A38" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F38" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I38" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="J38" t="s" s="2">
-        <v>263</v>
-      </c>
-      <c r="K38" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P38" s="2"/>
-      <c r="Q38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE38" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="AF38" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG38" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="AH38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ38" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>267</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK38">
+  <autoFilter ref="A1:AK25">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5049,7 +3478,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI37">
+  <conditionalFormatting sqref="A2:AI24">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>